<commit_message>
updated the fresh on packing edit page with pripority in filling and production page
</commit_message>
<xml_diff>
--- a/Production_plan_2.0.xlsx
+++ b/Production_plan_2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanjay.Khadka\GB_APP\GB-APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063CFC2F-3C7E-46A5-82F9-3B098FEF83F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4BAFF6-F6A2-4067-8557-DF89B6298B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="2430" windowWidth="24195" windowHeight="12675" xr2:uid="{F0426719-BCD1-4476-9DD7-17D1E3D05C92}"/>
+    <workbookView xWindow="240" yWindow="1470" windowWidth="24630" windowHeight="12675" xr2:uid="{F0426719-BCD1-4476-9DD7-17D1E3D05C92}"/>
   </bookViews>
   <sheets>
     <sheet name="soh_table" sheetId="1" r:id="rId1"/>
@@ -2178,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD08828-E480-4E05-80E4-AD92D6750B94}">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B180"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>